<commit_message>
Update [Launch testnet] Airdrop List.xlsx
</commit_message>
<xml_diff>
--- a/airdrop/[Launch testnet] Airdrop List.xlsx
+++ b/airdrop/[Launch testnet] Airdrop List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/data/sales/airdrop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C0280EA-81BB-BF47-8E82-AB1DDF23CAAE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0642460B-D6FD-AF4C-87EB-274AD94944A5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -223,11 +223,11 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -451,21 +451,21 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="117" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="7.5" style="6" customWidth="1"/>
-    <col min="2" max="2" width="23.6640625" style="6" customWidth="1"/>
-    <col min="3" max="3" width="34.33203125" style="6" customWidth="1"/>
-    <col min="4" max="4" width="19.6640625" style="7" customWidth="1"/>
-    <col min="5" max="5" width="51.1640625" style="6" customWidth="1"/>
-    <col min="6" max="6" width="45.5" style="6" customWidth="1"/>
-    <col min="7" max="16384" width="14.5" style="6"/>
+    <col min="1" max="1" width="7.5" style="5" customWidth="1"/>
+    <col min="2" max="2" width="23.6640625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="34.33203125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="51.1640625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="45.5" style="5" customWidth="1"/>
+    <col min="7" max="16384" width="14.5" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="6" customFormat="1" ht="15.75" customHeight="1">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -482,242 +482,242 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="6" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-    </row>
-    <row r="3" spans="1:5" s="6" customFormat="1" ht="15.75" customHeight="1">
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+    </row>
+    <row r="3" spans="1:5" ht="15.75" customHeight="1">
       <c r="A3" s="2">
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>33</v>
       </c>
       <c r="D3" s="3">
         <v>500</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="6" customFormat="1" ht="15.75" customHeight="1">
+    <row r="4" spans="1:5" ht="15.75" customHeight="1">
       <c r="A4" s="2">
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="5" t="s">
         <v>34</v>
       </c>
       <c r="D4" s="3">
         <v>100</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="6" customFormat="1" ht="15.75" customHeight="1">
+    <row r="5" spans="1:5" ht="15.75" customHeight="1">
       <c r="A5" s="2">
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="5" t="s">
         <v>35</v>
       </c>
       <c r="D5" s="3">
         <v>100</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="6" customFormat="1" ht="15.75" customHeight="1">
+    <row r="6" spans="1:5" ht="15.75" customHeight="1">
       <c r="A6" s="2">
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="5" t="s">
         <v>36</v>
       </c>
       <c r="D6" s="3">
         <v>100</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="6" customFormat="1" ht="15.75" customHeight="1">
+    <row r="7" spans="1:5" ht="15.75" customHeight="1">
       <c r="A7" s="2">
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="5" t="s">
         <v>37</v>
       </c>
       <c r="D7" s="3">
         <v>100</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="6" customFormat="1" ht="15.75" customHeight="1">
+    <row r="8" spans="1:5" ht="15.75" customHeight="1">
       <c r="A8" s="2">
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="5" t="s">
         <v>38</v>
       </c>
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="6" customFormat="1" ht="15.75" customHeight="1">
+    <row r="9" spans="1:5" ht="15.75" customHeight="1">
       <c r="A9" s="2">
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="5" t="s">
         <v>39</v>
       </c>
       <c r="D9" s="3">
         <v>100</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="E9" s="5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="6" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A10" s="5" t="s">
+    <row r="10" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A10" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-    </row>
-    <row r="11" spans="1:5" s="6" customFormat="1" ht="15.75" customHeight="1">
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+    </row>
+    <row r="11" spans="1:5" ht="15.75" customHeight="1">
       <c r="A11" s="4">
         <v>1</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="5" t="s">
         <v>40</v>
       </c>
       <c r="D11" s="3">
         <v>100</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="E11" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:5" s="6" customFormat="1" ht="15.75" customHeight="1">
+    <row r="12" spans="1:5" ht="15.75" customHeight="1">
       <c r="A12" s="4">
         <v>2</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="5" t="s">
         <v>41</v>
       </c>
       <c r="D12" s="3">
         <v>100</v>
       </c>
-      <c r="E12" s="6" t="s">
+      <c r="E12" s="5" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:5" s="6" customFormat="1" ht="15.75" customHeight="1">
+    <row r="13" spans="1:5" ht="15.75" customHeight="1">
       <c r="A13" s="4">
         <v>3</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="5" t="s">
         <v>42</v>
       </c>
       <c r="D13" s="3">
         <v>100</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="E13" s="5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:5" s="6" customFormat="1" ht="15.75" customHeight="1">
+    <row r="14" spans="1:5" ht="15.75" customHeight="1">
       <c r="A14" s="4">
         <v>4</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="5" t="s">
         <v>43</v>
       </c>
       <c r="D14" s="3">
         <v>100</v>
       </c>
-      <c r="E14" s="6" t="s">
+      <c r="E14" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:5" s="6" customFormat="1" ht="15.75" customHeight="1">
+    <row r="15" spans="1:5" ht="15.75" customHeight="1">
       <c r="A15" s="4">
         <v>5</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="5" t="s">
         <v>44</v>
       </c>
       <c r="D15" s="3">
         <v>100</v>
       </c>
-      <c r="E15" s="6" t="s">
+      <c r="E15" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:5" s="6" customFormat="1" ht="15.75" customHeight="1">
+    <row r="16" spans="1:5" ht="15.75" customHeight="1">
       <c r="A16" s="4">
         <v>6</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="5" t="s">
         <v>45</v>
       </c>
       <c r="D16" s="3">
         <v>100</v>
       </c>
-      <c r="E16" s="6" t="s">
+      <c r="E16" s="5" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>